<commit_message>
updata test case Signed-off-by: MaHongTao <mht@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/已完成/test_契約管理_契約者一覧.xlsx
+++ b/test_物件管理/已完成/test_契約管理_契約者一覧.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340">
   <si>
     <t>SQL</t>
   </si>
@@ -3474,48 +3474,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>VIEW</t>
-  </si>
-  <si>
-    <t>v_whiteboard_position</t>
-  </si>
-  <si>
-    <t>whiteboard_id</t>
-  </si>
-  <si>
-    <t>position_status</t>
-  </si>
-  <si>
-    <t>contract_end_date</t>
-  </si>
-  <si>
-    <t>return_date</t>
-  </si>
-  <si>
-    <t>subscription_count</t>
-  </si>
-  <si>
-    <t>empty_date</t>
-  </si>
-  <si>
-    <t>東京都大田区中央8-20-12</t>
-  </si>
-  <si>
-    <t>東京都大田区蒲田4-20-9</t>
-  </si>
-  <si>
-    <t>東京都板橋区小茂根1-20-8</t>
-  </si>
-  <si>
-    <t>東京都板橋区坂下1-33-21</t>
-  </si>
-  <si>
-    <t>東京都大田区蒲田5-21-5</t>
-  </si>
-  <si>
-    <t>東京都江戸川区西葛西8-4-6</t>
-  </si>
-  <si>
     <t>URL:</t>
   </si>
   <si>
@@ -4114,15 +4072,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4262,46 +4219,8 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4315,6 +4234,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -4323,7 +4264,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4338,7 +4279,53 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -4359,43 +4346,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -4404,10 +4354,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4516,7 +4466,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4534,7 +4580,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4546,139 +4628,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4742,26 +4692,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4781,37 +4731,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4834,6 +4764,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -4845,10 +4795,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="36" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4857,19 +4807,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4878,117 +4828,117 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5110,8 +5060,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="50">
@@ -5558,10 +5506,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:IE367"/>
+  <dimension ref="A2:IE346"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="L348" sqref="L348"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="M332" sqref="M332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -52869,1615 +52817,81 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="328" ht="14.25" spans="3:4">
-      <c r="C328" s="14" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D328" s="9" t="s">
-        <v>1143</v>
-      </c>
+    <row r="328" ht="12.75" spans="3:4">
+      <c r="C328" s="48"/>
+      <c r="D328" s="48"/>
     </row>
-    <row r="329" spans="4:4">
-      <c r="D329" s="17" t="s">
-        <v>1123</v>
-      </c>
+    <row r="329" ht="12.75" spans="3:4">
+      <c r="C329" s="48"/>
+      <c r="D329" s="48"/>
     </row>
-    <row r="330" ht="12.75" spans="4:32">
-      <c r="D330" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="E330" s="49" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F330" s="49" t="s">
-        <v>371</v>
-      </c>
-      <c r="G330" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H330" s="49" t="s">
-        <v>271</v>
-      </c>
-      <c r="I330" s="49" t="s">
-        <v>278</v>
-      </c>
-      <c r="J330" s="49" t="s">
-        <v>235</v>
-      </c>
-      <c r="K330" s="49" t="s">
-        <v>1145</v>
-      </c>
-      <c r="L330" s="49" t="s">
-        <v>1146</v>
-      </c>
-      <c r="M330" s="49" t="s">
-        <v>1147</v>
-      </c>
-      <c r="N330" s="49" t="s">
-        <v>1148</v>
-      </c>
-      <c r="O330" s="49" t="s">
-        <v>1149</v>
-      </c>
-      <c r="P330" s="49" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q330" s="49" t="s">
-        <v>255</v>
-      </c>
-      <c r="R330" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="S330" s="49" t="s">
-        <v>257</v>
-      </c>
-      <c r="T330" s="49" t="s">
-        <v>258</v>
-      </c>
-      <c r="U330" s="49" t="s">
-        <v>259</v>
-      </c>
-      <c r="V330" s="49" t="s">
-        <v>260</v>
-      </c>
-      <c r="W330" s="49" t="s">
-        <v>261</v>
-      </c>
-      <c r="X330" s="49" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y330" s="49" t="s">
-        <v>263</v>
-      </c>
-      <c r="Z330" s="49" t="s">
-        <v>264</v>
-      </c>
-      <c r="AA330" s="49" t="s">
-        <v>265</v>
-      </c>
-      <c r="AB330" s="49" t="s">
-        <v>266</v>
-      </c>
-      <c r="AC330" s="49" t="s">
-        <v>267</v>
-      </c>
-      <c r="AD330" s="49" t="s">
-        <v>268</v>
-      </c>
-      <c r="AE330" s="49" t="s">
-        <v>269</v>
-      </c>
-      <c r="AF330" s="49" t="s">
-        <v>272</v>
-      </c>
+    <row r="330" ht="12.75" spans="3:4">
+      <c r="C330" s="48"/>
+      <c r="D330" s="48"/>
     </row>
-    <row r="331" ht="12.75" spans="4:32">
-      <c r="D331" s="28">
-        <v>390</v>
-      </c>
-      <c r="E331" s="28">
-        <v>105027</v>
-      </c>
-      <c r="F331" s="28">
-        <v>390</v>
-      </c>
-      <c r="G331" s="28">
-        <v>394</v>
-      </c>
-      <c r="H331" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J331" s="28" t="s">
-        <v>1150</v>
-      </c>
-      <c r="K331" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L331" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N331" s="28">
-        <v>0</v>
-      </c>
-      <c r="O331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P331" s="28">
-        <v>19800</v>
-      </c>
-      <c r="Q331" s="28">
-        <v>18857</v>
-      </c>
-      <c r="R331" s="28">
-        <v>20520</v>
-      </c>
-      <c r="S331" s="28">
-        <v>19000</v>
-      </c>
-      <c r="T331" s="28">
-        <v>14580</v>
-      </c>
-      <c r="U331" s="28">
-        <v>13500</v>
-      </c>
-      <c r="V331" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W331" s="28">
-        <v>1950</v>
-      </c>
-      <c r="X331" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y331" s="28">
-        <v>1500</v>
-      </c>
-      <c r="Z331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA331" s="28">
-        <v>1700</v>
-      </c>
-      <c r="AB331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE331" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF331" s="28">
-        <v>0</v>
-      </c>
+    <row r="331" ht="12.75" spans="3:4">
+      <c r="C331" s="48"/>
+      <c r="D331" s="48"/>
     </row>
-    <row r="332" ht="12.75" spans="4:32">
-      <c r="D332" s="28">
-        <v>15</v>
-      </c>
-      <c r="E332" s="28">
-        <v>123100</v>
-      </c>
-      <c r="F332" s="28">
-        <v>15</v>
-      </c>
-      <c r="G332" s="28">
-        <v>15</v>
-      </c>
-      <c r="H332" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J332" s="28" t="s">
-        <v>1151</v>
-      </c>
-      <c r="K332" s="28" t="s">
-        <v>605</v>
-      </c>
-      <c r="L332" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N332" s="28">
-        <v>0</v>
-      </c>
-      <c r="O332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P332" s="28">
-        <v>31500</v>
-      </c>
-      <c r="Q332" s="28">
-        <v>30000</v>
-      </c>
-      <c r="R332" s="28">
-        <v>32400</v>
-      </c>
-      <c r="S332" s="28">
-        <v>30000</v>
-      </c>
-      <c r="T332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="U332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="W332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="X332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE332" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF332" s="28">
-        <v>0</v>
-      </c>
+    <row r="332" ht="12.75" spans="3:4">
+      <c r="C332" s="48"/>
+      <c r="D332" s="48"/>
     </row>
-    <row r="333" ht="12.75" spans="4:32">
-      <c r="D333" s="28">
-        <v>1</v>
-      </c>
-      <c r="E333" s="28">
-        <v>123236</v>
-      </c>
-      <c r="F333" s="28">
-        <v>1</v>
-      </c>
-      <c r="G333" s="28">
-        <v>1</v>
-      </c>
-      <c r="H333" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J333" s="28" t="s">
-        <v>1152</v>
-      </c>
-      <c r="K333" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L333" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N333" s="28">
-        <v>0</v>
-      </c>
-      <c r="O333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P333" s="28">
-        <v>24800</v>
-      </c>
-      <c r="Q333" s="28">
-        <v>23619</v>
-      </c>
-      <c r="R333" s="28">
-        <v>24840</v>
-      </c>
-      <c r="S333" s="28">
-        <v>23000</v>
-      </c>
-      <c r="T333" s="28">
-        <v>17280</v>
-      </c>
-      <c r="U333" s="28">
-        <v>16000</v>
-      </c>
-      <c r="V333" s="28">
-        <v>4850</v>
-      </c>
-      <c r="W333" s="28">
-        <v>1850</v>
-      </c>
-      <c r="X333" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y333" s="28">
-        <v>1700</v>
-      </c>
-      <c r="Z333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE333" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF333" s="28">
-        <v>0</v>
-      </c>
+    <row r="333" ht="12.75" spans="3:4">
+      <c r="C333" s="48"/>
+      <c r="D333" s="48"/>
     </row>
-    <row r="334" ht="12.75" spans="4:32">
-      <c r="D334" s="28">
-        <v>2</v>
-      </c>
-      <c r="E334" s="28">
-        <v>123236</v>
-      </c>
-      <c r="F334" s="28">
-        <v>2</v>
-      </c>
-      <c r="G334" s="28">
-        <v>2</v>
-      </c>
-      <c r="H334" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J334" s="28" t="s">
-        <v>1152</v>
-      </c>
-      <c r="K334" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L334" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N334" s="28">
-        <v>0</v>
-      </c>
-      <c r="O334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P334" s="28">
-        <v>27800</v>
-      </c>
-      <c r="Q334" s="28">
-        <v>26476</v>
-      </c>
-      <c r="R334" s="28">
-        <v>25920</v>
-      </c>
-      <c r="S334" s="28">
-        <v>24000</v>
-      </c>
-      <c r="T334" s="28">
-        <v>19440</v>
-      </c>
-      <c r="U334" s="28">
-        <v>18000</v>
-      </c>
-      <c r="V334" s="28">
-        <v>4850</v>
-      </c>
-      <c r="W334" s="28">
-        <v>1850</v>
-      </c>
-      <c r="X334" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y334" s="28">
-        <v>1700</v>
-      </c>
-      <c r="Z334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE334" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF334" s="28">
-        <v>0</v>
-      </c>
+    <row r="334" ht="12.75" spans="3:4">
+      <c r="C334" s="48"/>
+      <c r="D334" s="48"/>
     </row>
-    <row r="335" ht="12.75" spans="4:32">
-      <c r="D335" s="28">
-        <v>3</v>
-      </c>
-      <c r="E335" s="28">
-        <v>123236</v>
-      </c>
-      <c r="F335" s="28">
-        <v>3</v>
-      </c>
-      <c r="G335" s="28">
-        <v>3</v>
-      </c>
-      <c r="H335" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J335" s="28" t="s">
-        <v>1152</v>
-      </c>
-      <c r="K335" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L335" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N335" s="28">
-        <v>0</v>
-      </c>
-      <c r="O335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R335" s="28">
-        <v>27000</v>
-      </c>
-      <c r="S335" s="28">
-        <v>25000</v>
-      </c>
-      <c r="T335" s="28">
-        <v>22680</v>
-      </c>
-      <c r="U335" s="28">
-        <v>21000</v>
-      </c>
-      <c r="V335" s="28">
-        <v>4850</v>
-      </c>
-      <c r="W335" s="28">
-        <v>1850</v>
-      </c>
-      <c r="X335" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y335" s="28">
-        <v>1700</v>
-      </c>
-      <c r="Z335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE335" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF335" s="28">
-        <v>0</v>
-      </c>
+    <row r="335" ht="12.75" spans="3:4">
+      <c r="C335" s="48"/>
+      <c r="D335" s="48"/>
     </row>
-    <row r="336" ht="12.75" spans="4:32">
-      <c r="D336" s="28">
-        <v>4</v>
-      </c>
-      <c r="E336" s="28">
-        <v>123236</v>
-      </c>
-      <c r="F336" s="28">
-        <v>4</v>
-      </c>
-      <c r="G336" s="28">
-        <v>4</v>
-      </c>
-      <c r="H336" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J336" s="28" t="s">
-        <v>1152</v>
-      </c>
-      <c r="K336" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L336" s="50">
-        <v>43373</v>
-      </c>
-      <c r="M336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N336" s="28">
-        <v>0</v>
-      </c>
-      <c r="O336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R336" s="28">
-        <v>28620</v>
-      </c>
-      <c r="S336" s="28">
-        <v>26500</v>
-      </c>
-      <c r="T336" s="28">
-        <v>15</v>
-      </c>
-      <c r="U336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V336" s="28">
-        <v>4850</v>
-      </c>
-      <c r="W336" s="28">
-        <v>1850</v>
-      </c>
-      <c r="X336" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y336" s="28">
-        <v>1700</v>
-      </c>
-      <c r="Z336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE336" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF336" s="28">
-        <v>0</v>
-      </c>
+    <row r="336" ht="12.75" spans="3:4">
+      <c r="C336" s="48"/>
+      <c r="D336" s="48"/>
     </row>
-    <row r="337" ht="12.75" spans="4:32">
-      <c r="D337" s="28">
-        <v>5</v>
-      </c>
-      <c r="E337" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F337" s="28">
-        <v>5</v>
-      </c>
-      <c r="G337" s="28">
-        <v>5</v>
-      </c>
-      <c r="H337" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J337" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K337" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L337" s="50">
-        <v>43373</v>
-      </c>
-      <c r="M337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N337" s="28">
-        <v>0</v>
-      </c>
-      <c r="O337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R337" s="28">
-        <v>21600</v>
-      </c>
-      <c r="S337" s="28">
-        <v>20000</v>
-      </c>
-      <c r="T337" s="28">
-        <v>18360</v>
-      </c>
-      <c r="U337" s="28">
-        <v>17000</v>
-      </c>
-      <c r="V337" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W337" s="28">
-        <v>1750</v>
-      </c>
-      <c r="X337" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y337" s="28">
-        <v>2000</v>
-      </c>
-      <c r="Z337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA337" s="28">
-        <v>1830</v>
-      </c>
-      <c r="AB337" s="28">
-        <v>120</v>
-      </c>
-      <c r="AC337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE337" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF337" s="28">
-        <v>0</v>
-      </c>
+    <row r="337" ht="12.75" spans="3:4">
+      <c r="C337" s="48"/>
+      <c r="D337" s="48"/>
     </row>
-    <row r="338" ht="12.75" spans="4:32">
-      <c r="D338" s="28">
-        <v>6</v>
-      </c>
-      <c r="E338" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F338" s="28">
-        <v>6</v>
-      </c>
-      <c r="G338" s="28">
-        <v>6</v>
-      </c>
-      <c r="H338" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J338" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K338" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N338" s="28">
-        <v>0</v>
-      </c>
-      <c r="O338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R338" s="28">
-        <v>23760</v>
-      </c>
-      <c r="S338" s="28">
-        <v>22000</v>
-      </c>
-      <c r="T338" s="28">
-        <v>19440</v>
-      </c>
-      <c r="U338" s="28">
-        <v>18000</v>
-      </c>
-      <c r="V338" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W338" s="28">
-        <v>1750</v>
-      </c>
-      <c r="X338" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y338" s="28">
-        <v>2000</v>
-      </c>
-      <c r="Z338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA338" s="28">
-        <v>1830</v>
-      </c>
-      <c r="AB338" s="28">
-        <v>120</v>
-      </c>
-      <c r="AC338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE338" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF338" s="28">
-        <v>0</v>
-      </c>
+    <row r="338" ht="12.75" spans="3:4">
+      <c r="C338" s="48"/>
+      <c r="D338" s="48"/>
     </row>
-    <row r="339" ht="12.75" spans="4:32">
-      <c r="D339" s="28">
-        <v>7</v>
-      </c>
-      <c r="E339" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F339" s="28">
-        <v>7</v>
-      </c>
-      <c r="G339" s="28">
-        <v>7</v>
-      </c>
-      <c r="H339" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J339" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K339" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N339" s="28">
-        <v>0</v>
-      </c>
-      <c r="O339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R339" s="28">
-        <v>21600</v>
-      </c>
-      <c r="S339" s="28">
-        <v>20000</v>
-      </c>
-      <c r="T339" s="28">
-        <v>18360</v>
-      </c>
-      <c r="U339" s="28">
-        <v>17000</v>
-      </c>
-      <c r="V339" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W339" s="28">
-        <v>1750</v>
-      </c>
-      <c r="X339" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y339" s="28">
-        <v>2000</v>
-      </c>
-      <c r="Z339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA339" s="28">
-        <v>1830</v>
-      </c>
-      <c r="AB339" s="28">
-        <v>120</v>
-      </c>
-      <c r="AC339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE339" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF339" s="28">
-        <v>0</v>
-      </c>
+    <row r="339" ht="12.75" spans="3:4">
+      <c r="C339" s="48"/>
+      <c r="D339" s="48"/>
     </row>
-    <row r="340" ht="12.75" spans="4:32">
-      <c r="D340" s="28">
-        <v>8</v>
-      </c>
-      <c r="E340" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F340" s="28">
-        <v>8</v>
-      </c>
-      <c r="G340" s="28">
-        <v>8</v>
-      </c>
-      <c r="H340" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J340" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K340" s="28" t="s">
-        <v>1118</v>
-      </c>
-      <c r="L340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N340" s="28">
-        <v>1</v>
-      </c>
-      <c r="O340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R340" s="28">
-        <v>23760</v>
-      </c>
-      <c r="S340" s="28">
-        <v>22000</v>
-      </c>
-      <c r="T340" s="28">
-        <v>18360</v>
-      </c>
-      <c r="U340" s="28">
-        <v>17000</v>
-      </c>
-      <c r="V340" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W340" s="28">
-        <v>1750</v>
-      </c>
-      <c r="X340" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y340" s="28">
-        <v>2000</v>
-      </c>
-      <c r="Z340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA340" s="28">
-        <v>1830</v>
-      </c>
-      <c r="AB340" s="28">
-        <v>120</v>
-      </c>
-      <c r="AC340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE340" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF340" s="28">
-        <v>0</v>
-      </c>
+    <row r="340" ht="12.75" spans="3:4">
+      <c r="C340" s="48"/>
+      <c r="D340" s="48"/>
     </row>
-    <row r="341" ht="12.75" spans="4:32">
-      <c r="D341" s="28">
-        <v>9</v>
-      </c>
-      <c r="E341" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F341" s="28">
-        <v>9</v>
-      </c>
-      <c r="G341" s="28">
-        <v>9</v>
-      </c>
-      <c r="H341" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J341" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K341" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N341" s="28">
-        <v>0</v>
-      </c>
-      <c r="O341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R341" s="28">
-        <v>25920</v>
-      </c>
-      <c r="S341" s="28">
-        <v>24000</v>
-      </c>
-      <c r="T341" s="28">
-        <v>21600</v>
-      </c>
-      <c r="U341" s="28">
-        <v>20000</v>
-      </c>
-      <c r="V341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="W341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="X341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE341" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF341" s="28">
-        <v>0</v>
-      </c>
+    <row r="341" ht="12.75" spans="3:4">
+      <c r="C341" s="48"/>
+      <c r="D341" s="48"/>
     </row>
-    <row r="342" ht="12.75" spans="4:32">
-      <c r="D342" s="28">
-        <v>10</v>
-      </c>
-      <c r="E342" s="28">
-        <v>123295</v>
-      </c>
-      <c r="F342" s="28">
-        <v>10</v>
-      </c>
-      <c r="G342" s="28">
-        <v>10</v>
-      </c>
-      <c r="H342" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J342" s="28" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K342" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="L342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N342" s="28">
-        <v>0</v>
-      </c>
-      <c r="O342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R342" s="28">
-        <v>27000</v>
-      </c>
-      <c r="S342" s="28">
-        <v>25000</v>
-      </c>
-      <c r="T342" s="28">
-        <v>21600</v>
-      </c>
-      <c r="U342" s="28">
-        <v>20000</v>
-      </c>
-      <c r="V342" s="28">
-        <v>4700</v>
-      </c>
-      <c r="W342" s="28">
-        <v>1750</v>
-      </c>
-      <c r="X342" s="28">
-        <v>1550</v>
-      </c>
-      <c r="Y342" s="28">
-        <v>2000</v>
-      </c>
-      <c r="Z342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA342" s="28">
-        <v>1830</v>
-      </c>
-      <c r="AB342" s="28">
-        <v>120</v>
-      </c>
-      <c r="AC342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE342" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF342" s="28">
-        <v>0</v>
-      </c>
+    <row r="342" ht="12.75" spans="3:4">
+      <c r="C342" s="48"/>
+      <c r="D342" s="48"/>
     </row>
-    <row r="343" ht="12.75" spans="4:32">
-      <c r="D343" s="28">
-        <v>12</v>
-      </c>
-      <c r="E343" s="28">
-        <v>123372</v>
-      </c>
-      <c r="F343" s="28">
-        <v>12</v>
-      </c>
-      <c r="G343" s="28">
-        <v>12</v>
-      </c>
-      <c r="H343" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J343" s="28" t="s">
-        <v>1150</v>
-      </c>
-      <c r="K343" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="L343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N343" s="28">
-        <v>0</v>
-      </c>
-      <c r="O343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R343" s="28">
-        <v>29160</v>
-      </c>
-      <c r="S343" s="28">
-        <v>27000</v>
-      </c>
-      <c r="T343" s="28">
-        <v>27000</v>
-      </c>
-      <c r="U343" s="28">
-        <v>25000</v>
-      </c>
-      <c r="V343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="W343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="X343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE343" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF343" s="28">
-        <v>0</v>
-      </c>
+    <row r="343" ht="12.75" spans="3:4">
+      <c r="C343" s="48"/>
+      <c r="D343" s="48"/>
     </row>
-    <row r="344" ht="12.75" spans="4:32">
-      <c r="D344" s="28">
-        <v>13</v>
-      </c>
-      <c r="E344" s="28">
-        <v>123372</v>
-      </c>
-      <c r="F344" s="28">
-        <v>13</v>
-      </c>
-      <c r="G344" s="28">
-        <v>13</v>
-      </c>
-      <c r="H344" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J344" s="28" t="s">
-        <v>1150</v>
-      </c>
-      <c r="K344" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="L344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N344" s="28">
-        <v>0</v>
-      </c>
-      <c r="O344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R344" s="28">
-        <v>29160</v>
-      </c>
-      <c r="S344" s="28">
-        <v>27000</v>
-      </c>
-      <c r="T344" s="28">
-        <v>16200</v>
-      </c>
-      <c r="U344" s="28">
-        <v>15000</v>
-      </c>
-      <c r="V344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="W344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="X344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE344" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF344" s="28">
-        <v>0</v>
-      </c>
+    <row r="344" ht="12.75" spans="3:4">
+      <c r="C344" s="48"/>
+      <c r="D344" s="48"/>
     </row>
-    <row r="345" ht="12.75" spans="4:32">
-      <c r="D345" s="28">
-        <v>14</v>
-      </c>
-      <c r="E345" s="28">
-        <v>123373</v>
-      </c>
-      <c r="F345" s="28">
-        <v>14</v>
-      </c>
-      <c r="G345" s="28">
-        <v>14</v>
-      </c>
-      <c r="H345" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J345" s="28" t="s">
-        <v>1154</v>
-      </c>
-      <c r="K345" s="28" t="s">
-        <v>605</v>
-      </c>
-      <c r="L345" s="50">
-        <v>43343</v>
-      </c>
-      <c r="M345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N345" s="28">
-        <v>0</v>
-      </c>
-      <c r="O345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R345" s="28">
-        <v>5400</v>
-      </c>
-      <c r="S345" s="28">
-        <v>5000</v>
-      </c>
-      <c r="T345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="U345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="W345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="X345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE345" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF345" s="28">
-        <v>0</v>
-      </c>
+    <row r="345" ht="12.75" spans="3:4">
+      <c r="C345" s="48"/>
+      <c r="D345" s="48"/>
     </row>
-    <row r="346" ht="12.75" spans="4:32">
-      <c r="D346" s="28">
-        <v>11</v>
-      </c>
-      <c r="E346" s="28">
-        <v>123374</v>
-      </c>
-      <c r="F346" s="28">
-        <v>11</v>
-      </c>
-      <c r="G346" s="28">
-        <v>11</v>
-      </c>
-      <c r="H346" s="28">
-        <v>1001</v>
-      </c>
-      <c r="I346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J346" s="28" t="s">
-        <v>1155</v>
-      </c>
-      <c r="K346" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="L346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="M346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N346" s="28">
-        <v>0</v>
-      </c>
-      <c r="O346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R346" s="28">
-        <v>28620</v>
-      </c>
-      <c r="S346" s="28">
-        <v>26500</v>
-      </c>
-      <c r="T346" s="28">
-        <v>22680</v>
-      </c>
-      <c r="U346" s="28">
-        <v>21000</v>
-      </c>
-      <c r="V346" s="28">
-        <v>5000</v>
-      </c>
-      <c r="W346" s="28">
-        <v>1800</v>
-      </c>
-      <c r="X346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE346" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF346" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" ht="12.75" spans="4:5">
-      <c r="D347" s="48"/>
-      <c r="E347" s="48"/>
-    </row>
-    <row r="348" ht="12.75" spans="3:4">
-      <c r="C348" s="48"/>
-      <c r="D348" s="48"/>
-    </row>
-    <row r="349" ht="12.75" spans="3:4">
-      <c r="C349" s="48"/>
-      <c r="D349" s="48"/>
-    </row>
-    <row r="350" ht="12.75" spans="3:4">
-      <c r="C350" s="48"/>
-      <c r="D350" s="48"/>
-    </row>
-    <row r="351" ht="12.75" spans="3:4">
-      <c r="C351" s="48"/>
-      <c r="D351" s="48"/>
-    </row>
-    <row r="352" ht="12.75" spans="3:4">
-      <c r="C352" s="48"/>
-      <c r="D352" s="48"/>
-    </row>
-    <row r="353" ht="12.75" spans="3:4">
-      <c r="C353" s="48"/>
-      <c r="D353" s="48"/>
-    </row>
-    <row r="354" ht="12.75" spans="3:4">
-      <c r="C354" s="48"/>
-      <c r="D354" s="48"/>
-    </row>
-    <row r="355" ht="12.75" spans="3:4">
-      <c r="C355" s="48"/>
-      <c r="D355" s="48"/>
-    </row>
-    <row r="356" ht="12.75" spans="3:4">
-      <c r="C356" s="48"/>
-      <c r="D356" s="48"/>
-    </row>
-    <row r="357" ht="12.75" spans="3:4">
-      <c r="C357" s="48"/>
-      <c r="D357" s="48"/>
-    </row>
-    <row r="358" ht="12.75" spans="3:4">
-      <c r="C358" s="48"/>
-      <c r="D358" s="48"/>
-    </row>
-    <row r="359" ht="12.75" spans="3:4">
-      <c r="C359" s="48"/>
-      <c r="D359" s="48"/>
-    </row>
-    <row r="360" ht="12.75" spans="3:4">
-      <c r="C360" s="48"/>
-      <c r="D360" s="48"/>
-    </row>
-    <row r="361" ht="12.75" spans="3:4">
-      <c r="C361" s="48"/>
-      <c r="D361" s="48"/>
-    </row>
-    <row r="362" ht="12.75" spans="3:4">
-      <c r="C362" s="48"/>
-      <c r="D362" s="48"/>
-    </row>
-    <row r="363" ht="12.75" spans="3:4">
-      <c r="C363" s="48"/>
-      <c r="D363" s="48"/>
-    </row>
-    <row r="364" ht="12.75" spans="3:4">
-      <c r="C364" s="48"/>
-      <c r="D364" s="48"/>
-    </row>
-    <row r="365" ht="12.75" spans="3:4">
-      <c r="C365" s="48"/>
-      <c r="D365" s="48"/>
-    </row>
-    <row r="366" ht="12.75" spans="3:4">
-      <c r="C366" s="48"/>
-      <c r="D366" s="48"/>
-    </row>
-    <row r="367" ht="12.75" spans="3:4">
-      <c r="C367" s="48"/>
-      <c r="D367" s="48"/>
+    <row r="346" ht="12.75" spans="3:4">
+      <c r="C346" s="48"/>
+      <c r="D346" s="48"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B161">
@@ -54680,16 +53094,6 @@
       <formula>"NULL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C328">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"NULL"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D329">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NULL"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F231:F249">
     <cfRule type="cellIs" dxfId="0" priority="92" operator="equal">
       <formula>"NULL"</formula>
@@ -54870,7 +53274,7 @@
       <formula>"NULL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="$A1:$XFD90 $A324:$XFD327 $A99:$XFD160 A161 C161:XFD161 A348:B367 EQ206:XFD209 $A162:$XFD198 C199:XFD199 E348:XFD367 EM223 ES223:XFD223 $A368:$XFD1048576 E306:XFD306 C305:XFD305 $A302:$XFD303 N307:XFD323 A304:B304 E304:XFD304 A307:A323 L297:XFD301 C296:XFD296 A296:A301 B295:XFD295 $A291:$XFD294 K289:XFD290 C288:XFD288 A288:A290 B287:XFD287 $A285:$XFD286 A257:EL257 AC260:EL260 C258:EL259 A282:EL284 EM252:XFD284 EN229:XFD229 EM224:XFD228 B347:C347 AG330:XFD346 C330:C346 E328:XFD329 F347:XFD347">
+  <conditionalFormatting sqref="$A1:$XFD90 $A324:$XFD327 $A99:$XFD160 A161 C161:XFD161 EM224:XFD228 EN229:XFD229 EQ206:XFD209 $A162:$XFD198 C199:XFD199 EM252:XFD284 A282:EL284 EM223 ES223:XFD223 C258:EL259 E306:XFD306 C305:XFD305 $A302:$XFD303 N307:XFD323 A304:B304 E304:XFD304 A307:A323 L297:XFD301 C296:XFD296 A296:A301 B295:XFD295 $A291:$XFD294 K289:XFD290 C288:XFD288 A288:A290 B287:XFD287 $A285:$XFD286 A257:EL257 AC260:EL260 A328:B346 E328:XFD346 $A347:$XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="475" operator="equal">
       <formula>"NULL"</formula>
     </cfRule>
@@ -54970,11 +53374,6 @@
       <formula>"NULL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D328 C329">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"NULL"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -55002,37 +53401,37 @@
   <sheetData>
     <row r="1" s="9" customFormat="1" customHeight="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>1157</v>
+        <v>1142</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1143</v>
       </c>
       <c r="C1" s="11"/>
     </row>
     <row r="4" s="9" customFormat="1" customHeight="1" spans="1:3">
       <c r="A4" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1159</v>
+        <v>1145</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A5" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>1160</v>
+        <v>1146</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="7" customFormat="1" ht="14.25" spans="1:4">
       <c r="A7" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>1162</v>
+        <v>1148</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>1033</v>
@@ -55041,91 +53440,91 @@
     </row>
     <row r="8" customFormat="1" ht="14.25" spans="1:4">
       <c r="A8" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>1163</v>
+        <v>1149</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="9"/>
     </row>
     <row r="9" customFormat="1" ht="14.25" spans="1:4">
       <c r="A9" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>1165</v>
+        <v>1151</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="9"/>
     </row>
     <row r="10" customFormat="1" ht="14.25" spans="1:4">
       <c r="A10" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>1162</v>
+        <v>1148</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>1166</v>
+        <v>1152</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="1" ht="14.25" spans="1:4">
       <c r="A11" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>1163</v>
+        <v>1149</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="9"/>
     </row>
     <row r="12" customFormat="1" ht="14.25" spans="1:4">
       <c r="A12" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>1165</v>
+        <v>1151</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="9"/>
     </row>
     <row r="13" customFormat="1" ht="14.25" spans="1:4">
       <c r="A13" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>1162</v>
+        <v>1148</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>1167</v>
+        <v>1153</v>
       </c>
       <c r="D13" s="9"/>
     </row>
     <row r="14" customFormat="1" ht="14.25" spans="1:4">
       <c r="A14" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>1163</v>
+        <v>1149</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" customFormat="1" ht="14.25" spans="1:4">
       <c r="A15" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1165</v>
+        <v>1151</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="9"/>
     </row>
     <row r="16" customFormat="1" ht="14.25" spans="1:4">
       <c r="A16" s="10" t="s">
-        <v>1168</v>
+        <v>1154</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="11"/>
@@ -55133,20 +53532,20 @@
     </row>
     <row r="17" customFormat="1" ht="14.25" spans="1:4">
       <c r="A17" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>1169</v>
+        <v>1155</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="9"/>
     </row>
     <row r="18" customFormat="1" ht="14.25" spans="1:4">
       <c r="A18" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1170</v>
+        <v>1156</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="9"/>
@@ -55159,10 +53558,10 @@
     </row>
     <row r="21" s="9" customFormat="1" customHeight="1" spans="1:3">
       <c r="A21" s="10" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B21" s="51" t="s">
-        <v>1157</v>
+        <v>1142</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>1143</v>
       </c>
       <c r="C21" s="11"/>
     </row>
@@ -55171,38 +53570,38 @@
     </row>
     <row r="23" s="9" customFormat="1" customHeight="1" spans="1:3">
       <c r="A23" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>1159</v>
+        <v>1145</v>
       </c>
       <c r="C23" s="11"/>
     </row>
     <row r="24" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A24" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>1160</v>
+        <v>1146</v>
       </c>
       <c r="C24" s="11"/>
     </row>
     <row r="25" customFormat="1" ht="14.25" spans="1:4">
       <c r="A25" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>1171</v>
+        <v>1157</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="9"/>
     </row>
     <row r="26" customFormat="1" ht="14.25" spans="1:4">
       <c r="A26" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>1172</v>
+        <v>1158</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="9"/>
@@ -55215,57 +53614,57 @@
     </row>
     <row r="28" customFormat="1" ht="14.25" spans="1:4">
       <c r="A28" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>1173</v>
+        <v>1159</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="9"/>
     </row>
     <row r="29" customFormat="1" ht="14.25" spans="1:4">
       <c r="A29" s="10" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>1161</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>1175</v>
       </c>
       <c r="D29" s="9"/>
     </row>
     <row r="30" customFormat="1" ht="14.25" spans="1:4">
       <c r="A30" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1176</v>
+        <v>1162</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="9"/>
     </row>
     <row r="31" customFormat="1" ht="14.25" spans="1:4">
       <c r="A31" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>1177</v>
+        <v>1163</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>1178</v>
+        <v>1164</v>
       </c>
       <c r="D31" s="9"/>
     </row>
     <row r="32" customFormat="1" ht="14.25" spans="1:4">
       <c r="A32" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>1179</v>
+        <v>1165</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>1180</v>
+        <v>1166</v>
       </c>
       <c r="D32" s="9"/>
     </row>
@@ -55277,40 +53676,40 @@
     </row>
     <row r="34" customFormat="1" ht="14.25" spans="1:4">
       <c r="A34" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>1181</v>
+        <v>1167</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="9"/>
     </row>
     <row r="35" customFormat="1" ht="14.25" spans="1:4">
       <c r="A35" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>1182</v>
+        <v>1168</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="9"/>
     </row>
     <row r="36" customFormat="1" ht="14.25" spans="1:4">
       <c r="A36" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>1183</v>
+        <v>1169</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="9"/>
     </row>
     <row r="37" customFormat="1" ht="14.25" spans="1:4">
       <c r="A37" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>1184</v>
+        <v>1170</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="9"/>
@@ -55335,47 +53734,47 @@
     </row>
     <row r="41" customFormat="1" ht="14.25" spans="1:4">
       <c r="A41" s="10" t="s">
-        <v>1156</v>
+        <v>1142</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1185</v>
+        <v>1171</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="9"/>
     </row>
     <row r="42" customFormat="1" ht="14.25" spans="1:4">
       <c r="A42" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>1171</v>
+        <v>1157</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="9"/>
     </row>
     <row r="43" customFormat="1" ht="14.25" spans="1:4">
       <c r="A43" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B43" t="s">
-        <v>1186</v>
+        <v>1172</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="9"/>
     </row>
     <row r="44" customFormat="1" ht="14.25" spans="1:4">
       <c r="A44" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B44" t="s">
-        <v>1187</v>
+        <v>1173</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="9"/>
     </row>
     <row r="45" customFormat="1" ht="14.25" spans="1:4">
       <c r="A45" s="10" t="s">
-        <v>1188</v>
+        <v>1174</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
@@ -55385,19 +53784,19 @@
     </row>
     <row r="46" customFormat="1" ht="14.25" spans="1:4">
       <c r="A46" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>1162</v>
+        <v>1148</v>
       </c>
       <c r="C46" t="s">
-        <v>1189</v>
+        <v>1175</v>
       </c>
       <c r="D46" s="9"/>
     </row>
     <row r="47" customFormat="1" ht="14.25" spans="1:4">
       <c r="A47" s="10" t="s">
-        <v>1190</v>
+        <v>1176</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="11"/>
@@ -55405,10 +53804,10 @@
     </row>
     <row r="48" customFormat="1" ht="14.25" spans="1:4">
       <c r="A48" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>1191</v>
+        <v>1177</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="9"/>
@@ -55421,27 +53820,27 @@
     </row>
     <row r="50" customFormat="1" ht="14.25" spans="1:4">
       <c r="A50" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>1192</v>
+        <v>1178</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="9"/>
     </row>
     <row r="51" customFormat="1" ht="14.25" spans="1:4">
       <c r="A51" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>1193</v>
+        <v>1179</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="9"/>
     </row>
     <row r="52" customFormat="1" ht="14.25" spans="1:4">
       <c r="A52" s="10" t="s">
-        <v>1188</v>
+        <v>1174</v>
       </c>
       <c r="B52" s="9">
         <v>0</v>
@@ -55456,38 +53855,38 @@
     </row>
     <row r="54" customFormat="1" ht="14.25" spans="1:4">
       <c r="A54" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B54" t="s">
-        <v>1194</v>
+        <v>1180</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="9"/>
     </row>
     <row r="55" customFormat="1" ht="14.25" spans="1:2">
       <c r="A55" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>1195</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="56" customFormat="1" ht="14.25" spans="1:4">
       <c r="A56" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B56" t="s">
-        <v>1196</v>
+        <v>1182</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="9"/>
     </row>
     <row r="57" customFormat="1" ht="14.25" spans="1:3">
       <c r="A57" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B57" t="s">
-        <v>1197</v>
+        <v>1183</v>
       </c>
       <c r="C57">
         <v>18000</v>
@@ -55495,7 +53894,7 @@
     </row>
     <row r="58" customFormat="1" ht="14.25" spans="1:3">
       <c r="A58" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B58" t="s">
         <v>108</v>
@@ -55506,32 +53905,32 @@
     </row>
     <row r="59" customFormat="1" ht="14.25" spans="1:3">
       <c r="A59" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B59" t="s">
         <v>73</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>1180</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="60" customFormat="1" ht="14.25" spans="1:3">
       <c r="A60" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>1198</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="61" customFormat="1" ht="14.25" spans="1:3">
       <c r="A61" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B61" t="s">
-        <v>1199</v>
+        <v>1185</v>
       </c>
       <c r="C61" t="s">
         <v>984</v>
@@ -55539,10 +53938,10 @@
     </row>
     <row r="62" customFormat="1" ht="14.25" spans="1:3">
       <c r="A62" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B62" t="s">
-        <v>1200</v>
+        <v>1186</v>
       </c>
       <c r="C62" t="s">
         <v>575</v>
@@ -55550,10 +53949,10 @@
     </row>
     <row r="63" customFormat="1" ht="14.25" spans="1:3">
       <c r="A63" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B63" t="s">
-        <v>1176</v>
+        <v>1162</v>
       </c>
       <c r="C63" t="s">
         <v>1001</v>
@@ -55562,32 +53961,32 @@
     <row r="64" customFormat="1" ht="13.5"/>
     <row r="65" customFormat="1" ht="14.25" spans="1:2">
       <c r="A65" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B65" t="s">
-        <v>1201</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="66" customFormat="1" ht="14.25" spans="1:2">
       <c r="A66" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>1202</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="67" customFormat="1" ht="13.5"/>
     <row r="68" ht="14.25" spans="1:2">
       <c r="A68" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B68" t="s">
-        <v>1187</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="69" customFormat="1" ht="14.25" spans="1:3">
       <c r="A69" s="10" t="s">
-        <v>1188</v>
+        <v>1174</v>
       </c>
       <c r="B69" s="9">
         <v>1</v>
@@ -55596,10 +53995,10 @@
     </row>
     <row r="70" customFormat="1" ht="14.25" spans="1:3">
       <c r="A70" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>1162</v>
+        <v>1148</v>
       </c>
       <c r="C70" t="s">
         <v>220</v>
@@ -55607,17 +54006,17 @@
     </row>
     <row r="71" customFormat="1" ht="14.25" spans="1:3">
       <c r="A71" s="10" t="s">
-        <v>1190</v>
+        <v>1176</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="11"/>
     </row>
     <row r="72" customFormat="1" ht="14.25" spans="1:3">
       <c r="A72" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>1191</v>
+        <v>1177</v>
       </c>
       <c r="C72" s="11"/>
     </row>
@@ -55643,25 +54042,25 @@
     </row>
     <row r="77" customFormat="1" ht="14.25" spans="1:3">
       <c r="A77" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>1192</v>
+        <v>1178</v>
       </c>
       <c r="C77" s="11"/>
     </row>
     <row r="78" customFormat="1" ht="13.5" spans="2:3">
       <c r="B78" s="9" t="s">
-        <v>1203</v>
+        <v>1189</v>
       </c>
       <c r="C78" s="11"/>
     </row>
     <row r="79" customFormat="1" ht="14.25" spans="1:3">
       <c r="A79" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>1193</v>
+        <v>1179</v>
       </c>
       <c r="C79" s="11"/>
     </row>
@@ -55672,7 +54071,7 @@
     </row>
     <row r="81" customFormat="1" ht="14.25" spans="1:3">
       <c r="A81" s="10" t="s">
-        <v>1188</v>
+        <v>1174</v>
       </c>
       <c r="B81" s="9">
         <v>0</v>
@@ -55686,10 +54085,10 @@
     </row>
     <row r="84" customFormat="1" ht="14.25" spans="1:4">
       <c r="A84" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B84" t="s">
-        <v>1201</v>
+        <v>1187</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="9"/>
@@ -55706,10 +54105,10 @@
     </row>
     <row r="87" customFormat="1" ht="14.25" spans="1:2">
       <c r="A87" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>1204</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="88" customFormat="1" ht="13.5"/>
@@ -56239,7 +54638,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>1205</v>
+        <v>1191</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -56482,7 +54881,7 @@
     <row r="4" s="9" customFormat="1" spans="1:239">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
-        <v>1206</v>
+        <v>1192</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -56749,19 +55148,19 @@
         <v>346</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>1207</v>
+        <v>1193</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>1208</v>
+        <v>1194</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>1209</v>
+        <v>1195</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>1210</v>
+        <v>1196</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>1211</v>
+        <v>1197</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
@@ -57007,10 +55406,10 @@
         <v>84</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>1212</v>
+        <v>1198</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>1213</v>
+        <v>1199</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>185</v>
@@ -57274,10 +55673,10 @@
         <v>84</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>1214</v>
+        <v>1200</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>1215</v>
+        <v>1201</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>185</v>
@@ -57541,10 +55940,10 @@
         <v>84</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>1167</v>
+        <v>1153</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>1216</v>
+        <v>1202</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>185</v>
@@ -57808,10 +56207,10 @@
         <v>84</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>1217</v>
+        <v>1203</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>1218</v>
+        <v>1204</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>185</v>
@@ -58075,10 +56474,10 @@
         <v>84</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>1219</v>
+        <v>1205</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1220</v>
+        <v>1206</v>
       </c>
       <c r="I10" s="20" t="s">
         <v>185</v>
@@ -58345,7 +56744,7 @@
         <v>31</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>1221</v>
+        <v>1207</v>
       </c>
       <c r="I11" s="20">
         <v>1</v>
@@ -58612,7 +57011,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>1222</v>
+        <v>1208</v>
       </c>
       <c r="I12" s="20">
         <v>1</v>
@@ -58879,7 +57278,7 @@
         <v>35</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>1223</v>
+        <v>1209</v>
       </c>
       <c r="I13" s="20">
         <v>1</v>
@@ -59146,7 +57545,7 @@
         <v>40</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>1224</v>
+        <v>1210</v>
       </c>
       <c r="I14" s="20">
         <v>1</v>
@@ -59413,7 +57812,7 @@
         <v>41</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>1225</v>
+        <v>1211</v>
       </c>
       <c r="I15" s="20">
         <v>1</v>
@@ -59680,7 +58079,7 @@
         <v>42</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>1226</v>
+        <v>1212</v>
       </c>
       <c r="I16" s="20">
         <v>1</v>
@@ -59947,7 +58346,7 @@
         <v>50</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>1227</v>
+        <v>1213</v>
       </c>
       <c r="I17" s="20">
         <v>1</v>
@@ -60214,7 +58613,7 @@
         <v>60</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>1228</v>
+        <v>1214</v>
       </c>
       <c r="I18" s="20">
         <v>1</v>
@@ -60481,7 +58880,7 @@
         <v>61</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>1229</v>
+        <v>1215</v>
       </c>
       <c r="I19" s="20">
         <v>1</v>
@@ -61455,7 +59854,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>1230</v>
+        <v>1216</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="22"/>
@@ -61698,7 +60097,7 @@
     <row r="24" spans="1:239">
       <c r="A24" s="16"/>
       <c r="B24" s="17" t="s">
-        <v>1231</v>
+        <v>1217</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -61956,10 +60355,10 @@
         <v>67</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>1232</v>
+        <v>1218</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>1233</v>
+        <v>1219</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>108</v>
@@ -61968,7 +60367,7 @@
         <v>346</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>1234</v>
+        <v>1220</v>
       </c>
       <c r="L25" s="19" t="s">
         <v>1068</v>
@@ -61980,118 +60379,118 @@
         <v>371</v>
       </c>
       <c r="O25" s="19" t="s">
+        <v>1221</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>1222</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>1223</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>1224</v>
+      </c>
+      <c r="S25" s="19" t="s">
+        <v>1225</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>1226</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>1227</v>
+      </c>
+      <c r="V25" s="19" t="s">
+        <v>1228</v>
+      </c>
+      <c r="W25" s="19" t="s">
+        <v>1229</v>
+      </c>
+      <c r="X25" s="19" t="s">
+        <v>1230</v>
+      </c>
+      <c r="Y25" s="19" t="s">
+        <v>1231</v>
+      </c>
+      <c r="Z25" s="19" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AA25" s="19" t="s">
+        <v>1233</v>
+      </c>
+      <c r="AB25" s="19" t="s">
+        <v>1234</v>
+      </c>
+      <c r="AC25" s="19" t="s">
         <v>1235</v>
       </c>
-      <c r="P25" s="19" t="s">
+      <c r="AD25" s="19" t="s">
         <v>1236</v>
       </c>
-      <c r="Q25" s="19" t="s">
+      <c r="AE25" s="19" t="s">
         <v>1237</v>
       </c>
-      <c r="R25" s="19" t="s">
+      <c r="AF25" s="19" t="s">
         <v>1238</v>
       </c>
-      <c r="S25" s="19" t="s">
+      <c r="AG25" s="19" t="s">
         <v>1239</v>
       </c>
-      <c r="T25" s="19" t="s">
+      <c r="AH25" s="19" t="s">
         <v>1240</v>
       </c>
-      <c r="U25" s="19" t="s">
+      <c r="AI25" s="19" t="s">
         <v>1241</v>
       </c>
-      <c r="V25" s="19" t="s">
+      <c r="AJ25" s="19" t="s">
         <v>1242</v>
       </c>
-      <c r="W25" s="19" t="s">
+      <c r="AK25" s="19" t="s">
         <v>1243</v>
       </c>
-      <c r="X25" s="19" t="s">
+      <c r="AL25" s="19" t="s">
         <v>1244</v>
       </c>
-      <c r="Y25" s="19" t="s">
+      <c r="AM25" s="19" t="s">
         <v>1245</v>
       </c>
-      <c r="Z25" s="19" t="s">
+      <c r="AN25" s="19" t="s">
         <v>1246</v>
       </c>
-      <c r="AA25" s="19" t="s">
+      <c r="AO25" s="19" t="s">
         <v>1247</v>
       </c>
-      <c r="AB25" s="19" t="s">
+      <c r="AP25" s="19" t="s">
         <v>1248</v>
       </c>
-      <c r="AC25" s="19" t="s">
+      <c r="AQ25" s="19" t="s">
         <v>1249</v>
       </c>
-      <c r="AD25" s="19" t="s">
+      <c r="AR25" s="19" t="s">
         <v>1250</v>
       </c>
-      <c r="AE25" s="19" t="s">
+      <c r="AS25" s="19" t="s">
         <v>1251</v>
       </c>
-      <c r="AF25" s="19" t="s">
+      <c r="AT25" s="19" t="s">
         <v>1252</v>
       </c>
-      <c r="AG25" s="19" t="s">
+      <c r="AU25" s="19" t="s">
         <v>1253</v>
       </c>
-      <c r="AH25" s="19" t="s">
+      <c r="AV25" s="19" t="s">
         <v>1254</v>
       </c>
-      <c r="AI25" s="19" t="s">
+      <c r="AW25" s="19" t="s">
         <v>1255</v>
       </c>
-      <c r="AJ25" s="19" t="s">
+      <c r="AX25" s="19" t="s">
         <v>1256</v>
       </c>
-      <c r="AK25" s="19" t="s">
+      <c r="AY25" s="19" t="s">
         <v>1257</v>
       </c>
-      <c r="AL25" s="19" t="s">
+      <c r="AZ25" s="19" t="s">
         <v>1258</v>
-      </c>
-      <c r="AM25" s="19" t="s">
-        <v>1259</v>
-      </c>
-      <c r="AN25" s="19" t="s">
-        <v>1260</v>
-      </c>
-      <c r="AO25" s="19" t="s">
-        <v>1261</v>
-      </c>
-      <c r="AP25" s="19" t="s">
-        <v>1262</v>
-      </c>
-      <c r="AQ25" s="19" t="s">
-        <v>1263</v>
-      </c>
-      <c r="AR25" s="19" t="s">
-        <v>1264</v>
-      </c>
-      <c r="AS25" s="19" t="s">
-        <v>1265</v>
-      </c>
-      <c r="AT25" s="19" t="s">
-        <v>1266</v>
-      </c>
-      <c r="AU25" s="19" t="s">
-        <v>1267</v>
-      </c>
-      <c r="AV25" s="19" t="s">
-        <v>1268</v>
-      </c>
-      <c r="AW25" s="19" t="s">
-        <v>1269</v>
-      </c>
-      <c r="AX25" s="19" t="s">
-        <v>1270</v>
-      </c>
-      <c r="AY25" s="19" t="s">
-        <v>1271</v>
-      </c>
-      <c r="AZ25" s="19" t="s">
-        <v>1272</v>
       </c>
       <c r="BA25" s="19"/>
       <c r="BB25" s="23"/>
@@ -62284,7 +60683,7 @@
     <row r="26" spans="1:239">
       <c r="A26" s="13"/>
       <c r="B26" s="20" t="s">
-        <v>1273</v>
+        <v>1259</v>
       </c>
       <c r="C26" s="21">
         <v>43263.2788310185</v>
@@ -62299,16 +60698,16 @@
         <v>84</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>1274</v>
+        <v>1260</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>1275</v>
+        <v>1261</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>1095</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>1276</v>
+        <v>1262</v>
       </c>
       <c r="K26" s="20" t="s">
         <v>84</v>
@@ -62407,13 +60806,13 @@
         <v>84</v>
       </c>
       <c r="AQ26" s="20" t="s">
-        <v>1277</v>
+        <v>1263</v>
       </c>
       <c r="AR26" s="20" t="s">
-        <v>1278</v>
+        <v>1264</v>
       </c>
       <c r="AS26" s="20" t="s">
-        <v>1279</v>
+        <v>1265</v>
       </c>
       <c r="AT26" s="20" t="s">
         <v>84</v>
@@ -63111,7 +61510,7 @@
         <v>59</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>1280</v>
+        <v>1266</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="13"/>
@@ -63354,7 +61753,7 @@
     <row r="30" spans="1:239">
       <c r="A30" s="16"/>
       <c r="B30" s="17" t="s">
-        <v>1281</v>
+        <v>1267</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -63690,19 +62089,19 @@
         <v>407</v>
       </c>
       <c r="AG31" s="19" t="s">
-        <v>1243</v>
+        <v>1229</v>
       </c>
       <c r="AH31" s="19" t="s">
-        <v>1245</v>
+        <v>1231</v>
       </c>
       <c r="AI31" s="19" t="s">
-        <v>1244</v>
+        <v>1230</v>
       </c>
       <c r="AJ31" s="19" t="s">
         <v>1068</v>
       </c>
       <c r="AK31" s="19" t="s">
-        <v>1282</v>
+        <v>1268</v>
       </c>
       <c r="AL31" s="19" t="s">
         <v>270</v>
@@ -63711,172 +62110,172 @@
         <v>371</v>
       </c>
       <c r="AN31" s="19" t="s">
-        <v>1209</v>
+        <v>1195</v>
       </c>
       <c r="AO31" s="19" t="s">
-        <v>1283</v>
+        <v>1269</v>
       </c>
       <c r="AP31" s="19" t="s">
         <v>421</v>
       </c>
       <c r="AQ31" s="19" t="s">
-        <v>1284</v>
+        <v>1270</v>
       </c>
       <c r="AR31" s="19" t="s">
         <v>365</v>
       </c>
       <c r="AS31" s="19" t="s">
-        <v>1246</v>
+        <v>1232</v>
       </c>
       <c r="AT31" s="19" t="s">
-        <v>1247</v>
+        <v>1233</v>
       </c>
       <c r="AU31" s="19" t="s">
-        <v>1248</v>
+        <v>1234</v>
       </c>
       <c r="AV31" s="19" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AW31" s="19" t="s">
+        <v>1236</v>
+      </c>
+      <c r="AX31" s="19" t="s">
+        <v>1237</v>
+      </c>
+      <c r="AY31" s="19" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AZ31" s="19" t="s">
+        <v>1239</v>
+      </c>
+      <c r="BA31" s="19" t="s">
+        <v>1240</v>
+      </c>
+      <c r="BB31" s="19" t="s">
+        <v>1241</v>
+      </c>
+      <c r="BC31" s="19" t="s">
+        <v>1242</v>
+      </c>
+      <c r="BD31" s="19" t="s">
+        <v>1243</v>
+      </c>
+      <c r="BE31" s="19" t="s">
+        <v>1271</v>
+      </c>
+      <c r="BF31" s="19" t="s">
+        <v>1272</v>
+      </c>
+      <c r="BG31" s="19" t="s">
+        <v>1273</v>
+      </c>
+      <c r="BH31" s="19" t="s">
         <v>1249</v>
       </c>
-      <c r="AW31" s="19" t="s">
+      <c r="BI31" s="19" t="s">
         <v>1250</v>
       </c>
-      <c r="AX31" s="19" t="s">
+      <c r="BJ31" s="19" t="s">
         <v>1251</v>
       </c>
-      <c r="AY31" s="19" t="s">
+      <c r="BK31" s="19" t="s">
+        <v>1274</v>
+      </c>
+      <c r="BL31" s="19" t="s">
+        <v>1275</v>
+      </c>
+      <c r="BM31" s="19" t="s">
+        <v>1257</v>
+      </c>
+      <c r="BN31" s="19" t="s">
+        <v>1258</v>
+      </c>
+      <c r="BO31" s="19" t="s">
+        <v>1276</v>
+      </c>
+      <c r="BP31" s="19" t="s">
+        <v>1277</v>
+      </c>
+      <c r="BQ31" s="19" t="s">
+        <v>1278</v>
+      </c>
+      <c r="BR31" s="19" t="s">
+        <v>1279</v>
+      </c>
+      <c r="BS31" s="19" t="s">
+        <v>1280</v>
+      </c>
+      <c r="BT31" s="19" t="s">
         <v>1252</v>
       </c>
-      <c r="AZ31" s="19" t="s">
+      <c r="BU31" s="19" t="s">
         <v>1253</v>
       </c>
-      <c r="BA31" s="19" t="s">
+      <c r="BV31" s="19" t="s">
+        <v>1281</v>
+      </c>
+      <c r="BW31" s="19" t="s">
         <v>1254</v>
       </c>
-      <c r="BB31" s="19" t="s">
-        <v>1255</v>
-      </c>
-      <c r="BC31" s="19" t="s">
-        <v>1256</v>
-      </c>
-      <c r="BD31" s="19" t="s">
-        <v>1257</v>
-      </c>
-      <c r="BE31" s="19" t="s">
+      <c r="BX31" s="19" t="s">
+        <v>1282</v>
+      </c>
+      <c r="BY31" s="19" t="s">
+        <v>1283</v>
+      </c>
+      <c r="BZ31" s="19" t="s">
+        <v>1284</v>
+      </c>
+      <c r="CA31" s="19" t="s">
         <v>1285</v>
       </c>
-      <c r="BF31" s="19" t="s">
+      <c r="CB31" s="19" t="s">
         <v>1286</v>
       </c>
-      <c r="BG31" s="19" t="s">
+      <c r="CC31" s="19" t="s">
         <v>1287</v>
       </c>
-      <c r="BH31" s="19" t="s">
-        <v>1263</v>
-      </c>
-      <c r="BI31" s="19" t="s">
-        <v>1264</v>
-      </c>
-      <c r="BJ31" s="19" t="s">
-        <v>1265</v>
-      </c>
-      <c r="BK31" s="19" t="s">
+      <c r="CD31" s="19" t="s">
         <v>1288</v>
       </c>
-      <c r="BL31" s="19" t="s">
+      <c r="CE31" s="19" t="s">
         <v>1289</v>
       </c>
-      <c r="BM31" s="19" t="s">
-        <v>1271</v>
-      </c>
-      <c r="BN31" s="19" t="s">
-        <v>1272</v>
-      </c>
-      <c r="BO31" s="19" t="s">
+      <c r="CF31" s="19" t="s">
         <v>1290</v>
       </c>
-      <c r="BP31" s="19" t="s">
+      <c r="CG31" s="19" t="s">
         <v>1291</v>
       </c>
-      <c r="BQ31" s="19" t="s">
+      <c r="CH31" s="19" t="s">
         <v>1292</v>
       </c>
-      <c r="BR31" s="19" t="s">
+      <c r="CI31" s="19" t="s">
         <v>1293</v>
       </c>
-      <c r="BS31" s="19" t="s">
+      <c r="CJ31" s="19" t="s">
         <v>1294</v>
       </c>
-      <c r="BT31" s="19" t="s">
-        <v>1266</v>
-      </c>
-      <c r="BU31" s="19" t="s">
-        <v>1267</v>
-      </c>
-      <c r="BV31" s="19" t="s">
+      <c r="CK31" s="19" t="s">
         <v>1295</v>
       </c>
-      <c r="BW31" s="19" t="s">
-        <v>1268</v>
-      </c>
-      <c r="BX31" s="19" t="s">
+      <c r="CL31" s="19" t="s">
         <v>1296</v>
       </c>
-      <c r="BY31" s="19" t="s">
+      <c r="CM31" s="19" t="s">
         <v>1297</v>
       </c>
-      <c r="BZ31" s="19" t="s">
+      <c r="CN31" s="19" t="s">
         <v>1298</v>
       </c>
-      <c r="CA31" s="19" t="s">
+      <c r="CO31" s="19" t="s">
         <v>1299</v>
       </c>
-      <c r="CB31" s="19" t="s">
+      <c r="CP31" s="19" t="s">
         <v>1300</v>
       </c>
-      <c r="CC31" s="19" t="s">
+      <c r="CQ31" s="19" t="s">
         <v>1301</v>
-      </c>
-      <c r="CD31" s="19" t="s">
-        <v>1302</v>
-      </c>
-      <c r="CE31" s="19" t="s">
-        <v>1303</v>
-      </c>
-      <c r="CF31" s="19" t="s">
-        <v>1304</v>
-      </c>
-      <c r="CG31" s="19" t="s">
-        <v>1305</v>
-      </c>
-      <c r="CH31" s="19" t="s">
-        <v>1306</v>
-      </c>
-      <c r="CI31" s="19" t="s">
-        <v>1307</v>
-      </c>
-      <c r="CJ31" s="19" t="s">
-        <v>1308</v>
-      </c>
-      <c r="CK31" s="19" t="s">
-        <v>1309</v>
-      </c>
-      <c r="CL31" s="19" t="s">
-        <v>1310</v>
-      </c>
-      <c r="CM31" s="19" t="s">
-        <v>1311</v>
-      </c>
-      <c r="CN31" s="19" t="s">
-        <v>1312</v>
-      </c>
-      <c r="CO31" s="19" t="s">
-        <v>1313</v>
-      </c>
-      <c r="CP31" s="19" t="s">
-        <v>1314</v>
-      </c>
-      <c r="CQ31" s="19" t="s">
-        <v>1315</v>
       </c>
       <c r="CR31" s="13"/>
       <c r="CS31" s="13"/>
@@ -64123,7 +62522,7 @@
         <v>647</v>
       </c>
       <c r="AK32" s="20" t="s">
-        <v>1275</v>
+        <v>1261</v>
       </c>
       <c r="AL32" s="20" t="s">
         <v>195</v>
@@ -64132,7 +62531,7 @@
         <v>90</v>
       </c>
       <c r="AN32" s="20" t="s">
-        <v>1273</v>
+        <v>1259</v>
       </c>
       <c r="AO32" s="20" t="s">
         <v>84</v>
@@ -64192,13 +62591,13 @@
         <v>84</v>
       </c>
       <c r="BH32" s="20" t="s">
-        <v>1277</v>
+        <v>1263</v>
       </c>
       <c r="BI32" s="20" t="s">
-        <v>1278</v>
+        <v>1264</v>
       </c>
       <c r="BJ32" s="20" t="s">
-        <v>1279</v>
+        <v>1265</v>
       </c>
       <c r="BK32" s="20" t="s">
         <v>84</v>
@@ -64498,10 +62897,10 @@
   <sheetData>
     <row r="1" customFormat="1" ht="14.25" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>1156</v>
+        <v>1142</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1185</v>
+        <v>1171</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -64526,29 +62925,29 @@
     </row>
     <row r="5" customFormat="1" ht="14.25" spans="1:4">
       <c r="A5" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>1316</v>
+        <v>1302</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A6" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>1317</v>
+        <v>1303</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A7" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>1318</v>
+        <v>1304</v>
       </c>
       <c r="C7" s="11"/>
     </row>
@@ -64583,10 +62982,10 @@
   <sheetData>
     <row r="1" customFormat="1" ht="14.25" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>1156</v>
+        <v>1142</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1185</v>
+        <v>1171</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -64611,20 +63010,20 @@
     </row>
     <row r="5" customFormat="1" ht="14.25" spans="1:4">
       <c r="A5" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>1316</v>
+        <v>1302</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A6" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>1319</v>
+        <v>1305</v>
       </c>
       <c r="C6" s="11"/>
     </row>
@@ -64633,22 +63032,22 @@
     </row>
     <row r="8" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A8" s="10" t="s">
-        <v>1320</v>
+        <v>1306</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>1321</v>
+        <v>1307</v>
       </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A9" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>1322</v>
+        <v>1308</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1323</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="14.25" spans="1:3">
@@ -64657,19 +63056,19 @@
     </row>
     <row r="11" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>1324</v>
+        <v>1310</v>
       </c>
       <c r="C11" s="11"/>
     </row>
     <row r="12" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A12" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>1325</v>
+        <v>1311</v>
       </c>
       <c r="C12" s="11"/>
     </row>
@@ -64679,19 +63078,19 @@
     </row>
     <row r="14" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A14" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>1326</v>
+        <v>1312</v>
       </c>
       <c r="C14" s="11"/>
     </row>
     <row r="15" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A15" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>1327</v>
+        <v>1313</v>
       </c>
       <c r="C15" s="11"/>
     </row>
@@ -64700,13 +63099,13 @@
     </row>
     <row r="17" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A17" s="10" t="s">
-        <v>1161</v>
+        <v>1147</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>1328</v>
+        <v>1314</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>1329</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="18" s="9" customFormat="1" ht="12" spans="3:3">
@@ -64714,10 +63113,10 @@
     </row>
     <row r="19" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>1158</v>
+        <v>1144</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>1330</v>
+        <v>1316</v>
       </c>
       <c r="C19" s="11"/>
     </row>
@@ -64726,10 +63125,10 @@
     </row>
     <row r="21" s="9" customFormat="1" ht="14.25" spans="1:3">
       <c r="A21" s="10" t="s">
-        <v>1164</v>
+        <v>1150</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1331</v>
+        <v>1317</v>
       </c>
       <c r="C21" s="11"/>
     </row>
@@ -64751,7 +63150,7 @@
   <dimension ref="B4:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -64768,100 +63167,100 @@
   <sheetData>
     <row r="4" spans="2:8">
       <c r="B4" s="3" t="s">
-        <v>1332</v>
+        <v>1318</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1333</v>
+        <v>1319</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1333</v>
+        <v>1319</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>1334</v>
+        <v>1320</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>1335</v>
+        <v>1321</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>1336</v>
+        <v>1322</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>1335</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="8" t="s">
-        <v>1337</v>
+        <v>1323</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1338</v>
+        <v>1324</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1339</v>
+        <v>1325</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1340</v>
+        <v>1326</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1341</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="8" t="s">
-        <v>1342</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="8" t="s">
-        <v>1343</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="8" t="s">
-        <v>1344</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="8" t="s">
-        <v>1345</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="8" t="s">
-        <v>1346</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="8" t="s">
-        <v>1347</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="8" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1340</v>
+        <v>1326</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="8" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1340</v>
+        <v>1326</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="14" spans="2:2">

</xml_diff>